<commit_message>
input all data of JS
</commit_message>
<xml_diff>
--- a/JS.xlsx
+++ b/JS.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C15EF748-06E6-45AB-85EF-79D18351EF52}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1CA266-11D7-440C-BE70-A8D18CB5CFA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -540,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH550"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="BG4" sqref="BG4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AK4" sqref="AK4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>